<commit_message>
Dewax Rehydrate H&E:  temperature control added via temps,  added alc_temp  added temp module check
 to be upg to version 12 after quicktemp and testing
</commit_message>
<xml_diff>
--- a/protocols/H and E/H&E staining v11.0.xslx.xlsx
+++ b/protocols/H and E/H&E staining v11.0.xslx.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
     <sheet name="Dewax_Rehydrate H&amp;E Layout" sheetId="1" r:id="rId4"/>
@@ -11,10 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <si>
-    <t>These values are from StainWorks now, and match the generated protocol.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
   <si>
     <t>Omni-Stainer module type</t>
   </si>
@@ -32,6 +29,9 @@
   </si>
   <si>
     <t>Rehydration</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
   <si>
     <t>Clarifying</t>
@@ -73,28 +73,7 @@
     <t>Sample 5</t>
   </si>
   <si>
-    <t>Sample 6</t>
-  </si>
-  <si>
-    <t>Sample 7</t>
-  </si>
-  <si>
-    <t>Sample 8</t>
-  </si>
-  <si>
     <t>C</t>
-  </si>
-  <si>
-    <t>Sample 9</t>
-  </si>
-  <si>
-    <t>Sample 10</t>
-  </si>
-  <si>
-    <t>Sample 11</t>
-  </si>
-  <si>
-    <t>Sample 12</t>
   </si>
   <si>
     <t>Tiprack</t>
@@ -127,7 +106,7 @@
     <t>Blueing reagent</t>
   </si>
   <si>
-    <t>Clarifying agent</t>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Eosin</t>
@@ -138,18 +117,15 @@
   <si>
     <t>Volume/Sample</t>
   </si>
-  <si>
-    <t xml:space="preserve">No</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts>
+  <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts>
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -161,11 +137,6 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <b val="1"/>
       <sz val="12"/>
       <color indexed="8"/>
@@ -174,12 +145,12 @@
     <font>
       <b val="1"/>
       <sz val="12"/>
-      <color indexed="12"/>
+      <color indexed="11"/>
       <name val="Arial"/>
     </font>
     <font>
       <sz val="12"/>
-      <color indexed="12"/>
+      <color indexed="11"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -210,7 +181,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills>
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,7 +196,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
+        <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -260,7 +231,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders>
+  <borders count="91">
     <border>
       <left/>
       <right/>
@@ -269,158 +240,163 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <right/>
+      <left style="thick">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
       <top style="medium">
         <color indexed="8"/>
       </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <bottom style="thick">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
       <top style="medium">
         <color indexed="8"/>
       </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="8"/>
+      <bottom style="thick">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thick">
+        <color indexed="10"/>
       </right>
       <top style="medium">
         <color indexed="8"/>
       </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top style="thin">
+      <bottom style="thick">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
         <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
         <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="9"/>
-      </right>
-      <top style="thin">
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thick">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thick">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thick">
         <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="9"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="9"/>
-      </left>
-      <right style="thin">
-        <color indexed="9"/>
-      </right>
-      <top style="thin">
-        <color indexed="9"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="9"/>
+      </right>
+      <top style="thick">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thick">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thick">
-        <color indexed="11"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="9"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="9"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="9"/>
-      </left>
-      <right style="thin">
-        <color indexed="9"/>
-      </right>
-      <top/>
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
       <bottom style="thin">
         <color indexed="9"/>
       </bottom>
@@ -435,66 +411,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thick">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thick">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thick">
-        <color indexed="11"/>
-      </right>
-      <top style="thick">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="9"/>
-      </right>
-      <top style="thin">
-        <color indexed="9"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="9"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -548,7 +464,7 @@
     </border>
     <border>
       <left style="thick">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
@@ -557,7 +473,7 @@
         <color indexed="8"/>
       </top>
       <bottom style="thick">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -572,7 +488,7 @@
         <color indexed="8"/>
       </top>
       <bottom style="thick">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -581,13 +497,13 @@
         <color indexed="8"/>
       </left>
       <right style="thick">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </right>
       <top style="thick">
         <color indexed="8"/>
       </top>
       <bottom style="thick">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -619,7 +535,7 @@
         <color indexed="9"/>
       </right>
       <top style="thick">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="14"/>
@@ -634,7 +550,7 @@
         <color indexed="9"/>
       </right>
       <top style="thick">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -666,7 +582,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top/>
       <bottom/>
@@ -674,7 +590,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top/>
@@ -1031,7 +947,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top/>
       <bottom style="thin">
@@ -1041,7 +957,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top style="thick">
@@ -1291,79 +1207,79 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="9"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
       </left>
       <right/>
       <top style="thin">
@@ -1407,7 +1323,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top/>
@@ -1417,7 +1333,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
         <color indexed="9"/>
@@ -1427,12 +1343,12 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1441,7 +1357,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1452,18 +1368,18 @@
         <color indexed="9"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1473,7 +1389,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs>
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1481,18 +1397,21 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1501,340 +1420,328 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="37" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="51" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="52" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="53" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="54" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="55" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="56" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="57" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="58" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="59" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="60" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="61" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="62" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="63" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="64" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="65" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="66" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="67" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="68" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="69" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="70" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="71" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="72" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="73" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="73" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="73" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="74" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="75" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="77" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="77" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="78" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="79" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="30" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="75" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="42" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="80" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="8" borderId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="79" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="51" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="52" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="54" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="57" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="58" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="59" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="60" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="61" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="62" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="63" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="64" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="65" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="66" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="67" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="68" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="69" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="70" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="71" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="72" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="73" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="74" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="75" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="77" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="78" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="78" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="78" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="80" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="79" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="80" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="83" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="7" borderId="85" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="85" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="8" borderId="85" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="84" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="85" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="85" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="83" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="85" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="84" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="87" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="88" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="89" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="86" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="87" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="88" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="89" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="90" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="91" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="92" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="93" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="94" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="95" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1855,10 +1762,10 @@
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffff0000"/>
       <rgbColor rgb="ff3f3f76"/>
       <rgbColor rgb="ffffcc99"/>
+      <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ff00b050"/>
       <rgbColor rgb="ffffff00"/>
       <rgbColor rgb="ff002060"/>
@@ -1885,10 +1792,10 @@
       <xdr:rowOff>29869</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>292099</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2951,7 +2858,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr/>
+  <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2978,776 +2885,769 @@
     <col min="22" max="16384" width="12.6719" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="23" customHeight="1">
+    <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5"/>
+      <c r="D1" t="s" s="4">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="6"/>
       <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="8"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
     </row>
     <row r="2" ht="18" customHeight="1">
-      <c r="A2" t="s" s="9">
-        <v>1</v>
-      </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="11">
-        <v>10</v>
-      </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
+      <c r="A2" t="s" s="10">
+        <v>2</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="13">
+        <v>5</v>
+      </c>
+      <c r="E2" s="14"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
     </row>
     <row r="3" ht="18" customHeight="1">
-      <c r="A3" t="s" s="16">
+      <c r="A3" t="s" s="10">
         <v>3</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="18"/>
-      <c r="D3" t="s" s="19">
-        <v>42</v>
-      </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" t="s" s="17">
+        <v>4</v>
+      </c>
+      <c r="E3" s="14"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
     </row>
     <row r="4" ht="18" customHeight="1">
-      <c r="A4" t="s" s="16">
-        <v>4</v>
-      </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="18"/>
-      <c r="D4" t="s" s="22">
+      <c r="A4" t="s" s="10">
         <v>5</v>
       </c>
-      <c r="E4" s="20"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" t="s" s="17">
+        <v>6</v>
+      </c>
+      <c r="E4" s="14"/>
       <c r="F4" s="23"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
     </row>
     <row r="5" ht="18" customHeight="1">
-      <c r="A5" t="s" s="16">
-        <v>6</v>
-      </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="18"/>
-      <c r="D5" t="s" s="22">
-        <v>42</v>
-      </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="27"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
+      <c r="A5" t="s" s="10">
+        <v>7</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="24">
+        <v>150</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
     </row>
     <row r="6" ht="18" customHeight="1">
-      <c r="A6" t="s" s="16">
-        <v>7</v>
-      </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="22">
+      <c r="A6" t="s" s="25">
+        <v>8</v>
+      </c>
+      <c r="B6" s="26"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="28">
         <v>150</v>
       </c>
-      <c r="E6" s="20"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="27"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
     </row>
-    <row r="7" ht="18" customHeight="1">
-      <c r="A7" t="s" s="29">
-        <v>8</v>
-      </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="32">
-        <v>150</v>
-      </c>
-      <c r="E7" s="20"/>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="31"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="33"/>
       <c r="F7" s="33"/>
-      <c r="G7" s="34"/>
+      <c r="G7" s="33"/>
       <c r="H7" s="34"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="27"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="8"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="36"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="33"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="35"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="40"/>
-      <c r="O8" s="27"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="37"/>
+    <row r="8" ht="35" customHeight="1">
+      <c r="A8" t="s" s="37">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s" s="38">
+        <v>10</v>
+      </c>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="33"/>
+      <c r="S8" s="33"/>
+      <c r="T8" s="18"/>
+      <c r="U8" s="39"/>
     </row>
-    <row r="9" ht="35" customHeight="1">
-      <c r="A9" t="s" s="41">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s" s="42">
-        <v>10</v>
-      </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="37"/>
-      <c r="S9" s="37"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="43"/>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="40"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="33"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="20"/>
+      <c r="U9" s="39"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="44"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="46"/>
-      <c r="P10" s="37"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="25"/>
-      <c r="S10" s="25"/>
-      <c r="T10" s="25"/>
-      <c r="U10" s="43"/>
+      <c r="A10" t="s" s="43">
+        <v>11</v>
+      </c>
+      <c r="B10" s="44">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s" s="45">
+        <v>12</v>
+      </c>
+      <c r="D10" s="46"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="49"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="20"/>
+      <c r="U10" s="39"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" t="s" s="47">
-        <v>11</v>
-      </c>
-      <c r="B11" s="48">
+      <c r="A11" s="50"/>
+      <c r="B11" s="51">
+        <v>1</v>
+      </c>
+      <c r="C11" s="52">
         <v>2</v>
       </c>
-      <c r="C11" t="s" s="49">
-        <v>12</v>
-      </c>
-      <c r="D11" s="50"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="53"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="25"/>
-      <c r="R11" s="25"/>
-      <c r="S11" s="25"/>
-      <c r="T11" s="25"/>
-      <c r="U11" s="43"/>
+      <c r="D11" s="53">
+        <v>3</v>
+      </c>
+      <c r="E11" s="54">
+        <v>4</v>
+      </c>
+      <c r="F11" s="48"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="49"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="20"/>
+      <c r="T11" s="20"/>
+      <c r="U11" s="39"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="54"/>
-      <c r="B12" s="55">
-        <v>1</v>
-      </c>
-      <c r="C12" s="56">
-        <v>2</v>
-      </c>
-      <c r="D12" s="57">
-        <v>3</v>
-      </c>
-      <c r="E12" s="58">
-        <v>4</v>
-      </c>
-      <c r="F12" s="52"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="53"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="25"/>
-      <c r="T12" s="25"/>
-      <c r="U12" s="43"/>
+    <row r="12" ht="38" customHeight="1">
+      <c r="A12" t="s" s="55">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s" s="56">
+        <f>IF(B$11&lt;=$D$2,"Sample 1","")</f>
+        <v>14</v>
+      </c>
+      <c r="C12" t="s" s="57">
+        <f>IF(C$11&lt;=$D$2,"Sample 2","")</f>
+        <v>15</v>
+      </c>
+      <c r="D12" t="s" s="57">
+        <f>IF(D$11&lt;=$D$2,"Sample 3","")</f>
+        <v>16</v>
+      </c>
+      <c r="E12" t="s" s="58">
+        <f>IF(E$11&lt;=$D$2,"Sample 4","")</f>
+        <v>17</v>
+      </c>
+      <c r="F12" s="48"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="59"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="20"/>
+      <c r="U12" s="39"/>
     </row>
-    <row r="13" ht="38" customHeight="1">
-      <c r="A13" t="s" s="59">
-        <v>13</v>
-      </c>
-      <c r="B13" s="60">
-        <f>IF(B$12&lt;=$D$3,"Sample 1","")</f>
-      </c>
-      <c r="C13" s="61">
-        <f>IF(C$12&lt;=$D$3,"Sample 2","")</f>
-      </c>
-      <c r="D13" s="61">
-        <f>IF(D$12&lt;=$D$3,"Sample 3","")</f>
-      </c>
-      <c r="E13" s="62">
-        <f>IF(E$12&lt;=$D$3,"Sample 4","")</f>
-      </c>
-      <c r="F13" s="52"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="63"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="25"/>
-      <c r="R13" s="25"/>
-      <c r="S13" s="25"/>
-      <c r="T13" s="25"/>
-      <c r="U13" s="43"/>
+    <row r="13" ht="25" customHeight="1">
+      <c r="A13" t="s" s="55">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s" s="60">
+        <f>IF(B$11+4&lt;=$D$2,"Sample 5","")</f>
+        <v>19</v>
+      </c>
+      <c r="C13" t="s" s="61">
+        <f>IF(C$11+4&lt;=$D$2,"Sample 6","")</f>
+      </c>
+      <c r="D13" t="s" s="61">
+        <f>IF(D$11+4&lt;=$D$2,"Sample 7","")</f>
+      </c>
+      <c r="E13" t="s" s="62">
+        <f>IF(E$11+4&lt;=$D$2,"Sample 8","")</f>
+      </c>
+      <c r="F13" s="48"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="63"/>
+      <c r="O13" s="59"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="20"/>
+      <c r="S13" s="20"/>
+      <c r="T13" s="20"/>
+      <c r="U13" s="39"/>
     </row>
-    <row r="14" ht="25" customHeight="1">
-      <c r="A14" t="s" s="59">
-        <v>18</v>
-      </c>
-      <c r="B14" s="64">
-        <f>IF(B$12+4&lt;=$D$3,"Sample 5","")</f>
-      </c>
-      <c r="C14" s="65">
-        <f>IF(C$12+4&lt;=$D$3,"Sample 6","")</f>
-      </c>
-      <c r="D14" s="65">
-        <f>IF(D$12+4&lt;=$D$3,"Sample 7","")</f>
-      </c>
-      <c r="E14" s="66">
-        <f>IF(E$12+4&lt;=$D$3,"Sample 8","")</f>
-      </c>
-      <c r="F14" s="52"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="67"/>
-      <c r="O14" s="63"/>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="25"/>
-      <c r="R14" s="25"/>
-      <c r="S14" s="25"/>
-      <c r="T14" s="25"/>
-      <c r="U14" s="43"/>
+    <row r="14" ht="20" customHeight="1">
+      <c r="A14" t="s" s="64">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s" s="65">
+        <f>IF(B$11+8&lt;=$D$2,"Sample 9","")</f>
+      </c>
+      <c r="C14" t="s" s="66">
+        <f>IF(C$11+8&lt;=$D$2,"Sample 10","")</f>
+      </c>
+      <c r="D14" t="s" s="66">
+        <f>IF(D$11+8&lt;=$D$2,"Sample 11","")</f>
+      </c>
+      <c r="E14" t="s" s="67">
+        <f>IF(E$11+8&lt;=$D$2,"Sample 12","")</f>
+      </c>
+      <c r="F14" s="68"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="30"/>
+      <c r="R14" s="30"/>
+      <c r="S14" s="30"/>
+      <c r="T14" s="30"/>
+      <c r="U14" s="69"/>
     </row>
-    <row r="15" ht="20" customHeight="1">
-      <c r="A15" t="s" s="68">
-        <v>23</v>
-      </c>
-      <c r="B15" s="69">
-        <f>IF(B$12+8&lt;=$D$3,"Sample 9","")</f>
-      </c>
-      <c r="C15" s="70">
-        <f>IF(C$12+8&lt;=$D$3,"Sample 10","")</f>
-      </c>
-      <c r="D15" s="70">
-        <f>IF(D$12+8&lt;=$D$3,"Sample 11","")</f>
-      </c>
-      <c r="E15" s="71">
-        <f>IF(E$12+8&lt;=$D$3,"Sample 12","")</f>
-      </c>
-      <c r="F15" s="72"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="34"/>
-      <c r="O15" s="34"/>
-      <c r="P15" s="34"/>
-      <c r="Q15" s="34"/>
-      <c r="R15" s="34"/>
-      <c r="S15" s="34"/>
-      <c r="T15" s="34"/>
-      <c r="U15" s="73"/>
+    <row r="15" ht="13.5" customHeight="1">
+      <c r="A15" s="70"/>
+      <c r="B15" s="71"/>
+      <c r="C15" s="72"/>
+      <c r="D15" s="72"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="74"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
     </row>
-    <row r="16" ht="13.5" customHeight="1">
-      <c r="A16" s="74"/>
-      <c r="B16" s="75"/>
-      <c r="C16" s="76"/>
-      <c r="D16" s="76"/>
-      <c r="E16" s="77"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="78"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="8"/>
-      <c r="S16" s="8"/>
-      <c r="T16" s="8"/>
-      <c r="U16" s="8"/>
+    <row r="16" ht="26" customHeight="1">
+      <c r="A16" t="s" s="37">
+        <v>21</v>
+      </c>
+      <c r="B16" s="75">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s" s="76">
+        <v>22</v>
+      </c>
+      <c r="D16" s="77"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="79"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="74"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
     </row>
-    <row r="17" ht="26" customHeight="1">
-      <c r="A17" t="s" s="41">
-        <v>28</v>
-      </c>
-      <c r="B17" s="79">
-        <v>6</v>
-      </c>
-      <c r="C17" t="s" s="80">
-        <v>29</v>
-      </c>
-      <c r="D17" s="81"/>
-      <c r="E17" s="82"/>
-      <c r="F17" s="83"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="78"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
-      <c r="T17" s="8"/>
-      <c r="U17" s="8"/>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="40"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="80"/>
+      <c r="D17" s="80"/>
+      <c r="E17" s="80"/>
+      <c r="F17" s="81"/>
+      <c r="G17" s="82"/>
+      <c r="H17" s="83"/>
+      <c r="I17" s="83"/>
+      <c r="J17" s="83"/>
+      <c r="K17" s="83"/>
+      <c r="L17" s="84"/>
+      <c r="M17" s="85"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="44"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="84"/>
-      <c r="D18" s="84"/>
-      <c r="E18" s="84"/>
-      <c r="F18" s="85"/>
-      <c r="G18" s="86"/>
-      <c r="H18" s="87"/>
-      <c r="I18" s="87"/>
-      <c r="J18" s="87"/>
-      <c r="K18" s="87"/>
-      <c r="L18" s="88"/>
-      <c r="M18" s="89"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
-      <c r="R18" s="8"/>
-      <c r="S18" s="8"/>
-      <c r="T18" s="8"/>
-      <c r="U18" s="8"/>
+      <c r="A18" t="s" s="86">
+        <v>23</v>
+      </c>
+      <c r="B18" s="87">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s" s="88">
+        <v>24</v>
+      </c>
+      <c r="D18" s="89"/>
+      <c r="E18" s="90"/>
+      <c r="F18" s="90"/>
+      <c r="G18" s="90"/>
+      <c r="H18" s="90"/>
+      <c r="I18" s="90"/>
+      <c r="J18" s="90"/>
+      <c r="K18" s="90"/>
+      <c r="L18" s="90"/>
+      <c r="M18" s="91"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="9"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" t="s" s="90">
-        <v>30</v>
-      </c>
-      <c r="B19" s="91">
+      <c r="A19" s="92"/>
+      <c r="B19" s="93">
+        <v>1</v>
+      </c>
+      <c r="C19" s="94">
+        <v>2</v>
+      </c>
+      <c r="D19" s="94">
         <v>3</v>
       </c>
-      <c r="C19" t="s" s="92">
-        <v>31</v>
-      </c>
-      <c r="D19" s="93"/>
-      <c r="E19" s="94"/>
-      <c r="F19" s="94"/>
-      <c r="G19" s="94"/>
-      <c r="H19" s="94"/>
-      <c r="I19" s="94"/>
-      <c r="J19" s="94"/>
-      <c r="K19" s="94"/>
-      <c r="L19" s="94"/>
-      <c r="M19" s="95"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
-      <c r="Q19" s="8"/>
-      <c r="R19" s="8"/>
-      <c r="S19" s="8"/>
-      <c r="T19" s="8"/>
-      <c r="U19" s="8"/>
+      <c r="E19" s="94">
+        <v>4</v>
+      </c>
+      <c r="F19" s="94">
+        <v>5</v>
+      </c>
+      <c r="G19" s="94">
+        <v>6</v>
+      </c>
+      <c r="H19" s="95">
+        <v>7</v>
+      </c>
+      <c r="I19" s="95">
+        <v>8</v>
+      </c>
+      <c r="J19" s="95">
+        <v>9</v>
+      </c>
+      <c r="K19" s="95">
+        <v>10</v>
+      </c>
+      <c r="L19" s="96">
+        <v>11</v>
+      </c>
+      <c r="M19" s="97">
+        <v>12</v>
+      </c>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="96"/>
-      <c r="B20" s="97">
-        <v>1</v>
-      </c>
-      <c r="C20" s="98">
-        <v>2</v>
-      </c>
-      <c r="D20" s="98">
+      <c r="A20" t="s" s="98">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s" s="99">
+        <f>IF(D3="Yes","Dewax"," ")</f>
         <v>3</v>
       </c>
-      <c r="E20" s="98">
-        <v>4</v>
-      </c>
-      <c r="F20" s="98">
-        <v>5</v>
-      </c>
-      <c r="G20" s="98">
-        <v>6</v>
-      </c>
-      <c r="H20" s="99">
-        <v>7</v>
-      </c>
-      <c r="I20" s="99">
-        <v>8</v>
-      </c>
-      <c r="J20" s="99">
-        <v>9</v>
-      </c>
-      <c r="K20" s="99">
-        <v>10</v>
-      </c>
-      <c r="L20" s="100">
-        <v>11</v>
-      </c>
-      <c r="M20" s="101">
-        <v>12</v>
-      </c>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="8"/>
-      <c r="T20" s="8"/>
-      <c r="U20" s="8"/>
+      <c r="C20" t="s" s="99">
+        <v>25</v>
+      </c>
+      <c r="D20" t="s" s="99">
+        <v>26</v>
+      </c>
+      <c r="E20" t="s" s="99">
+        <v>27</v>
+      </c>
+      <c r="F20" t="s" s="99">
+        <v>28</v>
+      </c>
+      <c r="G20" t="s" s="99">
+        <v>29</v>
+      </c>
+      <c r="H20" t="s" s="99">
+        <v>30</v>
+      </c>
+      <c r="I20" t="s" s="99">
+        <f>IF(D5="Yes","Clarifying agent"," ")</f>
+        <v>31</v>
+      </c>
+      <c r="J20" s="100"/>
+      <c r="K20" s="100"/>
+      <c r="L20" t="s" s="101">
+        <v>32</v>
+      </c>
+      <c r="M20" s="102"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" t="s" s="102">
-        <v>13</v>
-      </c>
-      <c r="B21" s="103">
-        <f>IF(D4="Yes","Dewax"," ")</f>
-      </c>
-      <c r="C21" t="s" s="103">
-        <v>32</v>
-      </c>
-      <c r="D21" t="s" s="103">
+      <c r="A21" t="s" s="103">
         <v>33</v>
       </c>
-      <c r="E21" t="s" s="103">
-        <v>34</v>
-      </c>
-      <c r="F21" t="s" s="103">
-        <v>35</v>
-      </c>
-      <c r="G21" t="s" s="103">
-        <v>36</v>
-      </c>
-      <c r="H21" t="s" s="103">
-        <v>37</v>
-      </c>
-      <c r="I21" s="103">
-        <f>IF(D6="Yes","Clarifying agent"," ")</f>
-      </c>
-      <c r="J21" s="104"/>
-      <c r="K21" s="104"/>
-      <c r="L21" t="s" s="105">
-        <v>39</v>
-      </c>
-      <c r="M21" s="106"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="8"/>
-      <c r="R21" s="8"/>
-      <c r="S21" s="8"/>
-      <c r="T21" s="8"/>
-      <c r="U21" s="8"/>
+      <c r="B21" s="104">
+        <f>IF(D3="Yes",(B22*$D$2+2000)/1000," ")</f>
+        <v>3.5</v>
+      </c>
+      <c r="C21" s="104">
+        <f>(C22*$D$2+2000)/1000</f>
+        <v>7.25</v>
+      </c>
+      <c r="D21" s="104">
+        <f>(D22*$D$2+2000)/1000</f>
+        <v>4.25</v>
+      </c>
+      <c r="E21" s="104">
+        <f>(E22*$D$2+2000)/1000</f>
+        <v>3.5</v>
+      </c>
+      <c r="F21" s="104">
+        <f>(F22*$D$2+2000)/1000</f>
+        <v>8</v>
+      </c>
+      <c r="G21" s="104">
+        <f>(G22*$D$2+2000)/1000</f>
+        <v>3.5</v>
+      </c>
+      <c r="H21" s="104">
+        <f>(H22*$D$2+2000)/1000</f>
+        <v>2.75</v>
+      </c>
+      <c r="I21" t="s" s="105">
+        <f>IF(D5="Yes",(I22*$D$2+2000)/1000," ")</f>
+        <v>31</v>
+      </c>
+      <c r="J21" s="106"/>
+      <c r="K21" s="106"/>
+      <c r="L21" s="104">
+        <f>(L22*$D$2+2000)/1000</f>
+        <v>3.5</v>
+      </c>
+      <c r="M21" s="107"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" t="s" s="107">
-        <v>40</v>
-      </c>
-      <c r="B22" s="108">
-        <f>IF(D4="Yes",(B23*$D$3+2000)/1000," ")</f>
-      </c>
-      <c r="C22" s="108">
-        <f>(C23*$D$3+2000)/1000</f>
-      </c>
-      <c r="D22" s="108">
-        <f>(D23*$D$3+2000)/1000</f>
-      </c>
-      <c r="E22" s="108">
-        <f>(E23*$D$3+2000)/1000</f>
-      </c>
-      <c r="F22" s="108">
-        <f>(F23*$D$3+2000)/1000</f>
-      </c>
-      <c r="G22" s="108">
-        <f>(G23*$D$3+2000)/1000</f>
-      </c>
-      <c r="H22" s="108">
-        <f>(H23*$D$3+2000)/1000</f>
-      </c>
-      <c r="I22" s="108">
-        <f>IF(D6="Yes",(I23*$D$3+2000)/1000," ")</f>
-      </c>
-      <c r="J22" s="109"/>
-      <c r="K22" s="109"/>
-      <c r="L22" s="108">
-        <f>(L23*$D$3+2000)/1000</f>
-      </c>
-      <c r="M22" s="110"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
-      <c r="Q22" s="8"/>
-      <c r="R22" s="8"/>
-      <c r="S22" s="8"/>
-      <c r="T22" s="8"/>
-      <c r="U22" s="8"/>
+      <c r="A22" t="s" s="108">
+        <v>34</v>
+      </c>
+      <c r="B22" s="109">
+        <v>300</v>
+      </c>
+      <c r="C22" s="109">
+        <v>1050</v>
+      </c>
+      <c r="D22" s="109">
+        <v>450</v>
+      </c>
+      <c r="E22" s="109">
+        <v>300</v>
+      </c>
+      <c r="F22" s="110">
+        <v>1200</v>
+      </c>
+      <c r="G22" s="109">
+        <v>300</v>
+      </c>
+      <c r="H22" s="109">
+        <v>150</v>
+      </c>
+      <c r="I22" s="109">
+        <v>150</v>
+      </c>
+      <c r="J22" s="109">
+        <v>0</v>
+      </c>
+      <c r="K22" s="109">
+        <v>0</v>
+      </c>
+      <c r="L22" s="109">
+        <v>300</v>
+      </c>
+      <c r="M22" s="111">
+        <v>0</v>
+      </c>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" t="s" s="111">
-        <v>41</v>
-      </c>
-      <c r="B23" s="112">
-        <v>300</v>
-      </c>
-      <c r="C23" s="112">
-        <v>1050</v>
-      </c>
-      <c r="D23" s="112">
-        <v>450</v>
-      </c>
-      <c r="E23" s="112">
-        <v>300</v>
-      </c>
-      <c r="F23" s="113">
-        <v>1200</v>
-      </c>
-      <c r="G23" s="112">
-        <v>300</v>
-      </c>
-      <c r="H23" s="112">
-        <v>150</v>
-      </c>
-      <c r="I23" s="112">
-        <v>150</v>
-      </c>
-      <c r="J23" s="112">
-        <v>0</v>
-      </c>
-      <c r="K23" s="112">
-        <v>0</v>
-      </c>
-      <c r="L23" s="112">
-        <v>300</v>
-      </c>
-      <c r="M23" s="114">
-        <v>0</v>
-      </c>
-      <c r="N23" s="8"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
-      <c r="Q23" s="8"/>
-      <c r="R23" s="8"/>
-      <c r="S23" s="8"/>
-      <c r="T23" s="8"/>
-      <c r="U23" s="8"/>
+      <c r="A23" s="112"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="74"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="19"/>
+      <c r="Q23" s="19"/>
+      <c r="R23" s="19"/>
+      <c r="S23" s="19"/>
+      <c r="T23" s="19"/>
+      <c r="U23" s="113"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="115"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="78"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="78"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="23"/>
-      <c r="O24" s="24"/>
-      <c r="P24" s="24"/>
-      <c r="Q24" s="24"/>
-      <c r="R24" s="24"/>
-      <c r="S24" s="24"/>
-      <c r="T24" s="24"/>
-      <c r="U24" s="116"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="117"/>
-      <c r="B25" s="118"/>
-      <c r="C25" s="118"/>
-      <c r="D25" s="118"/>
-      <c r="E25" s="118"/>
-      <c r="F25" s="119"/>
-      <c r="G25" s="118"/>
-      <c r="H25" s="118"/>
-      <c r="I25" s="118"/>
-      <c r="J25" s="118"/>
-      <c r="K25" s="118"/>
-      <c r="L25" s="118"/>
-      <c r="M25" s="119"/>
-      <c r="N25" s="118"/>
-      <c r="O25" s="118"/>
-      <c r="P25" s="118"/>
-      <c r="Q25" s="118"/>
-      <c r="R25" s="118"/>
-      <c r="S25" s="118"/>
-      <c r="T25" s="118"/>
-      <c r="U25" s="120"/>
+      <c r="A24" s="114"/>
+      <c r="B24" s="115"/>
+      <c r="C24" s="115"/>
+      <c r="D24" s="115"/>
+      <c r="E24" s="115"/>
+      <c r="F24" s="116"/>
+      <c r="G24" s="115"/>
+      <c r="H24" s="115"/>
+      <c r="I24" s="115"/>
+      <c r="J24" s="115"/>
+      <c r="K24" s="115"/>
+      <c r="L24" s="115"/>
+      <c r="M24" s="116"/>
+      <c r="N24" s="115"/>
+      <c r="O24" s="115"/>
+      <c r="P24" s="115"/>
+      <c r="Q24" s="115"/>
+      <c r="R24" s="115"/>
+      <c r="S24" s="115"/>
+      <c r="T24" s="115"/>
+      <c r="U24" s="117"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A1:E1"/>
+  <mergeCells count="6">
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A5:C5"/>
     <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A5:C5"/>
   </mergeCells>
-  <dataValidations count="3">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1">
+      <formula1>"S12,C12,10"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
-      <formula1>"S12,C12"</formula1>
+      <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3">
-      <formula1>"1,2,3,4,5,6,7,8,9,10,11,12"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D4">
+      <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D6">
-      <formula1>"Yes,No"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5">
+      <formula1>"Yes,No,150"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>